<commit_message>
started adding navison process, needs more work
</commit_message>
<xml_diff>
--- a/Reiseregning/Redesignet prosess/Data/Config.xlsx
+++ b/Reiseregning/Redesignet prosess/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>Static part of logging message. Processed Transaction failed with application exception</t>
-  </si>
-  <si>
-    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
   </si>
   <si>
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
@@ -504,6 +501,18 @@
   </si>
   <si>
     <t>AditroQueue</t>
+  </si>
+  <si>
+    <t>NavisionQueueName</t>
+  </si>
+  <si>
+    <t>NavisionQueue</t>
+  </si>
+  <si>
+    <t>Aditro items Queue Name. Be sure to match this name with the one from the server.</t>
+  </si>
+  <si>
+    <t>Navision items Queue Name. Be sure to match this name with the one from the server.</t>
   </si>
 </sst>
 </file>
@@ -940,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -991,299 +1000,309 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="13" t="s">
+      <c r="C9" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="B11" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="C11" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="23" t="s">
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="B12" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="C12" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>97</v>
-      </c>
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="15"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>125</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="17" t="s">
+    </row>
+    <row r="20" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="B20" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>108</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>119</v>
+        <v>109</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>128</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="C23" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B28" s="3"/>
+        <v>63</v>
+      </c>
       <c r="C28" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="9"/>
+        <v>64</v>
+      </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="B30" s="9"/>
       <c r="C30" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="B32" s="11"/>
+      <c r="C32" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="C34" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2237,6 +2256,7 @@
     <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2353,35 +2373,35 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2455,13 +2475,13 @@
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
         <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2522,24 +2542,24 @@
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>